<commit_message>
Cust and Opt Finished
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2BD37F-256B-4E8B-8649-354B3A974399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EC064D-1271-4A46-A304-A6D1AF130ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="150">
   <si>
     <t>Product Name:</t>
   </si>
@@ -502,7 +502,7 @@
     <numFmt numFmtId="164" formatCode="mmm\ dd"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -565,6 +565,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -646,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -770,6 +776,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,19 +1002,19 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,25 +1302,25 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3666,8 +3675,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3686,7 +3695,7 @@
     <col min="12" max="1024" width="11.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3704,7 +3713,7 @@
       </c>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -3720,7 +3729,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3732,7 +3741,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -3750,7 +3759,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3765,12 +3774,16 @@
       <c r="H5" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="45">
         <v>1001942779</v>
       </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+    </row>
+    <row r="6" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -3782,7 +3795,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
@@ -3794,7 +3807,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
@@ -3806,7 +3819,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
@@ -3818,7 +3831,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -3830,7 +3843,7 @@
       <c r="I10"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -3850,7 +3863,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>0</v>
       </c>
@@ -3871,17 +3884,17 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>1</v>
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3895,13 +3908,13 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>2</v>
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 2")</f>
@@ -3919,13 +3932,13 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>3</v>
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 3")</f>
@@ -3943,13 +3956,13 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>4</v>
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -3969,7 +3982,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -4137,7 +4150,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -4169,7 +4182,9 @@
       <c r="F26" s="17">
         <v>1</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
       </c>
@@ -5344,7 +5359,8 @@
       <c r="K94" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="I5:N5"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="F22:G22"/>
@@ -5363,7 +5379,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Please enter your name as it appears in Blackboard." sqref="B5:B9" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Please enter your name as it appears in Blackboard." sqref="B5:B9 I5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5371,7 +5387,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Student ID" prompt="Please enter your UTA student ID number." sqref="I5:I9" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Student ID" prompt="Please enter your UTA student ID number." sqref="I6:I9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5422,8 +5438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5541,11 +5557,11 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -5559,7 +5575,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5577,7 +5593,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5595,7 +5611,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5613,7 +5629,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5631,7 +5647,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5649,7 +5665,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5701,7 +5717,7 @@
       <c r="C17" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="46" t="s">
         <v>141</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -5787,7 +5803,7 @@
         <v>145</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F22" s="38"/>
     </row>
@@ -5805,7 +5821,7 @@
         <v>147</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" s="38"/>
     </row>
@@ -5823,7 +5839,7 @@
         <v>148</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F24" s="38"/>
     </row>
@@ -5831,16 +5847,10 @@
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="39"/>
-      <c r="E25" s="37" t="s">
-        <v>144</v>
-      </c>
+      <c r="E25" s="37"/>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -6613,12 +6623,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>